<commit_message>
Implement create telegram instance to telegram process class.
</commit_message>
<xml_diff>
--- a/meta/program/BlancoRestGeneratorTsConstants.xlsx
+++ b/meta/program/BlancoRestGeneratorTsConstants.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoRestGeneratorTs/meta/program/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\t-narumi\Documents\project\Cacco\git\blancoRestGeneratorTs\meta\program\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0634CF2-3682-3147-B7A4-B0F068A19E2B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1000" yWindow="2700" windowWidth="21680" windowHeight="11060" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1005" yWindow="2700" windowWidth="21675" windowHeight="11055" tabRatio="640"/>
   </bookViews>
   <sheets>
     <sheet name="constants" sheetId="1" r:id="rId1"/>
@@ -33,7 +32,7 @@
     <definedName name="項目型">#REF!</definedName>
     <definedName name="必須">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -48,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="145">
   <si>
     <t>定数定義書</t>
   </si>
@@ -716,14 +715,36 @@
   </si>
   <si>
     <t>"Error"</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>java.lang.String</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>API_TELEGRAM_BASE</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>"ApiTelegram"</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>電文の基底クラス</t>
+    <rPh sb="0" eb="2">
+      <t>デンブン</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>キテイ</t>
+    </rPh>
     <phoneticPr fontId="4"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="ＭＳ Ｐゴシック"/>
@@ -1593,28 +1614,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H64"/>
+  <dimension ref="A1:H65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="D47" sqref="D47"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="D58" sqref="D58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="5" style="1" customWidth="1"/>
     <col min="2" max="2" width="29" style="1" customWidth="1"/>
-    <col min="3" max="3" width="26.6640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="27.33203125" style="1" customWidth="1"/>
-    <col min="5" max="6" width="22.1640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="33.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="26.625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="27.375" style="1" customWidth="1"/>
+    <col min="5" max="6" width="22.125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="33.375" style="1" customWidth="1"/>
     <col min="8" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="19">
+    <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1622,17 +1643,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
@@ -1640,7 +1661,7 @@
       <c r="C5" s="5"/>
       <c r="D5" s="6"/>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
@@ -1651,7 +1672,7 @@
       <c r="D6" s="9"/>
       <c r="E6" s="10"/>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
@@ -1662,7 +1683,7 @@
       <c r="D7" s="12"/>
       <c r="E7" s="10"/>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A8" s="4" t="s">
         <v>7</v>
       </c>
@@ -1674,7 +1695,7 @@
       <c r="E8" s="13"/>
       <c r="F8" s="9"/>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A9" s="4" t="s">
         <v>8</v>
       </c>
@@ -1685,7 +1706,7 @@
       <c r="D9"/>
       <c r="E9" s="15"/>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A10" s="16" t="s">
         <v>10</v>
       </c>
@@ -1696,7 +1717,7 @@
       <c r="D10" s="15"/>
       <c r="E10" s="15"/>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A11" s="16" t="s">
         <v>12</v>
       </c>
@@ -1705,7 +1726,7 @@
       <c r="D11" s="15"/>
       <c r="E11" s="15"/>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A12" s="16" t="s">
         <v>13</v>
       </c>
@@ -1714,14 +1735,14 @@
       <c r="D12" s="15"/>
       <c r="E12" s="15"/>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A13" s="15"/>
       <c r="B13" s="15"/>
       <c r="C13" s="15"/>
       <c r="D13" s="15"/>
       <c r="E13" s="15"/>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A14" s="4" t="s">
         <v>14</v>
       </c>
@@ -1730,7 +1751,7 @@
       <c r="D14" s="5"/>
       <c r="E14" s="6"/>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A15" s="16" t="s">
         <v>15</v>
       </c>
@@ -1739,7 +1760,7 @@
       <c r="D15" s="20"/>
       <c r="E15" s="21"/>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A16"/>
       <c r="B16"/>
       <c r="C16"/>
@@ -1747,7 +1768,7 @@
       <c r="E16"/>
       <c r="F16"/>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A17" s="4" t="s">
         <v>16</v>
       </c>
@@ -1759,7 +1780,7 @@
       <c r="G17"/>
       <c r="H17"/>
     </row>
-    <row r="18" spans="1:8" ht="13.5" customHeight="1">
+    <row r="18" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="43" t="s">
         <v>17</v>
       </c>
@@ -1779,7 +1800,7 @@
       <c r="G18"/>
       <c r="H18"/>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A19" s="43"/>
       <c r="B19" s="43"/>
       <c r="C19" s="44"/>
@@ -1789,7 +1810,7 @@
       <c r="G19"/>
       <c r="H19"/>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A20" s="24">
         <v>1</v>
       </c>
@@ -1809,7 +1830,7 @@
       <c r="G20"/>
       <c r="H20"/>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A21" s="24">
         <f>A20+1</f>
         <v>2</v>
@@ -1830,7 +1851,7 @@
       <c r="G21"/>
       <c r="H21"/>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A22" s="24">
         <f>A21+1</f>
         <v>3</v>
@@ -1851,9 +1872,9 @@
       <c r="G22"/>
       <c r="H22"/>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A23" s="24">
-        <f t="shared" ref="A23:A63" si="0">A22+1</f>
+        <f t="shared" ref="A23:A64" si="0">A22+1</f>
         <v>4</v>
       </c>
       <c r="B23" s="25" t="s">
@@ -1872,7 +1893,7 @@
       <c r="G23"/>
       <c r="H23"/>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A24" s="24">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1893,7 +1914,7 @@
       <c r="G24"/>
       <c r="H24"/>
     </row>
-    <row r="25" spans="1:8" s="42" customFormat="1">
+    <row r="25" spans="1:8" s="42" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A25" s="24">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1914,7 +1935,7 @@
       <c r="G25"/>
       <c r="H25"/>
     </row>
-    <row r="26" spans="1:8" s="42" customFormat="1">
+    <row r="26" spans="1:8" s="42" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A26" s="24">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1935,7 +1956,7 @@
       <c r="G26"/>
       <c r="H26"/>
     </row>
-    <row r="27" spans="1:8" s="42" customFormat="1">
+    <row r="27" spans="1:8" s="42" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A27" s="24">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1956,7 +1977,7 @@
       <c r="G27"/>
       <c r="H27"/>
     </row>
-    <row r="28" spans="1:8" s="42" customFormat="1">
+    <row r="28" spans="1:8" s="42" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A28" s="24">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1977,7 +1998,7 @@
       <c r="G28"/>
       <c r="H28"/>
     </row>
-    <row r="29" spans="1:8" s="42" customFormat="1">
+    <row r="29" spans="1:8" s="42" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A29" s="24">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1998,7 +2019,7 @@
       <c r="G29"/>
       <c r="H29"/>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A30" s="24">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -2019,7 +2040,7 @@
       <c r="G30"/>
       <c r="H30"/>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A31" s="24">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -2040,7 +2061,7 @@
       <c r="G31"/>
       <c r="H31"/>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A32" s="24">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -2061,7 +2082,7 @@
       <c r="G32"/>
       <c r="H32"/>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A33" s="24">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -2082,7 +2103,7 @@
       <c r="G33"/>
       <c r="H33"/>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A34" s="24">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -2103,7 +2124,7 @@
       <c r="G34"/>
       <c r="H34"/>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A35" s="24">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -2124,7 +2145,7 @@
       <c r="G35"/>
       <c r="H35"/>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A36" s="24">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -2145,7 +2166,7 @@
       <c r="G36"/>
       <c r="H36"/>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A37" s="24">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -2166,7 +2187,7 @@
       <c r="G37"/>
       <c r="H37"/>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A38" s="24">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -2187,7 +2208,7 @@
       <c r="G38"/>
       <c r="H38"/>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A39" s="24">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -2208,7 +2229,7 @@
       <c r="G39"/>
       <c r="H39"/>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A40" s="24">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -2229,7 +2250,7 @@
       <c r="G40"/>
       <c r="H40"/>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A41" s="24">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -2250,7 +2271,7 @@
       <c r="G41"/>
       <c r="H41"/>
     </row>
-    <row r="42" spans="1:8">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A42" s="24">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -2271,7 +2292,7 @@
       <c r="G42"/>
       <c r="H42"/>
     </row>
-    <row r="43" spans="1:8">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A43" s="24">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -2292,7 +2313,7 @@
       <c r="G43"/>
       <c r="H43"/>
     </row>
-    <row r="44" spans="1:8">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A44" s="24">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -2313,7 +2334,7 @@
       <c r="G44"/>
       <c r="H44"/>
     </row>
-    <row r="45" spans="1:8">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A45" s="24">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -2334,7 +2355,7 @@
       <c r="G45"/>
       <c r="H45"/>
     </row>
-    <row r="46" spans="1:8">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A46" s="24">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -2353,7 +2374,7 @@
       </c>
       <c r="F46" s="35"/>
     </row>
-    <row r="47" spans="1:8">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A47" s="24">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -2372,7 +2393,7 @@
       </c>
       <c r="F47" s="35"/>
     </row>
-    <row r="48" spans="1:8">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A48" s="24">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -2391,7 +2412,7 @@
       </c>
       <c r="F48" s="35"/>
     </row>
-    <row r="49" spans="1:8">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A49" s="24">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -2410,7 +2431,7 @@
       </c>
       <c r="F49" s="35"/>
     </row>
-    <row r="50" spans="1:8">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A50" s="24">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -2431,7 +2452,7 @@
       <c r="G50"/>
       <c r="H50"/>
     </row>
-    <row r="51" spans="1:8">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A51" s="24">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -2452,7 +2473,7 @@
       <c r="G51"/>
       <c r="H51"/>
     </row>
-    <row r="52" spans="1:8">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A52" s="24">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -2473,7 +2494,7 @@
       <c r="G52"/>
       <c r="H52"/>
     </row>
-    <row r="53" spans="1:8">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A53" s="24">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -2494,7 +2515,7 @@
       <c r="G53"/>
       <c r="H53"/>
     </row>
-    <row r="54" spans="1:8">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A54" s="24">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -2515,7 +2536,7 @@
       <c r="G54"/>
       <c r="H54"/>
     </row>
-    <row r="55" spans="1:8">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A55" s="24">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -2536,7 +2557,7 @@
       <c r="G55"/>
       <c r="H55"/>
     </row>
-    <row r="56" spans="1:8">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A56" s="24">
         <f t="shared" si="0"/>
         <v>37</v>
@@ -2557,7 +2578,7 @@
       <c r="G56"/>
       <c r="H56"/>
     </row>
-    <row r="57" spans="1:8">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A57" s="24">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -2578,7 +2599,7 @@
       <c r="G57"/>
       <c r="H57"/>
     </row>
-    <row r="58" spans="1:8">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A58" s="24">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -2599,7 +2620,7 @@
       <c r="G58"/>
       <c r="H58"/>
     </row>
-    <row r="59" spans="1:8">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A59" s="24">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -2620,7 +2641,7 @@
       <c r="G59"/>
       <c r="H59"/>
     </row>
-    <row r="60" spans="1:8">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A60" s="24">
         <f t="shared" si="0"/>
         <v>41</v>
@@ -2629,7 +2650,7 @@
         <v>124</v>
       </c>
       <c r="C60" s="34" t="s">
-        <v>33</v>
+        <v>141</v>
       </c>
       <c r="D60" s="34" t="s">
         <v>130</v>
@@ -2641,7 +2662,7 @@
       <c r="G60"/>
       <c r="H60"/>
     </row>
-    <row r="61" spans="1:8">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A61" s="24">
         <f t="shared" si="0"/>
         <v>42</v>
@@ -2662,7 +2683,7 @@
       <c r="G61"/>
       <c r="H61"/>
     </row>
-    <row r="62" spans="1:8">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A62" s="24">
         <f t="shared" si="0"/>
         <v>43</v>
@@ -2683,7 +2704,7 @@
       <c r="G62"/>
       <c r="H62"/>
     </row>
-    <row r="63" spans="1:8">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A63" s="24">
         <f t="shared" si="0"/>
         <v>44</v>
@@ -2704,15 +2725,36 @@
       <c r="G63"/>
       <c r="H63"/>
     </row>
-    <row r="64" spans="1:8">
-      <c r="A64" s="24"/>
-      <c r="B64" s="33"/>
-      <c r="C64" s="34"/>
-      <c r="D64" s="34"/>
-      <c r="E64" s="34"/>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A64" s="24">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="B64" s="33" t="s">
+        <v>142</v>
+      </c>
+      <c r="C64" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="D64" s="34" t="s">
+        <v>143</v>
+      </c>
+      <c r="E64" s="34" t="s">
+        <v>144</v>
+      </c>
       <c r="F64" s="35"/>
       <c r="G64"/>
       <c r="H64"/>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A65" s="24"/>
+      <c r="B65" s="33"/>
+      <c r="C65" s="34"/>
+      <c r="D65" s="34"/>
+      <c r="E65" s="34"/>
+      <c r="F65" s="35"/>
+      <c r="G65"/>
+      <c r="H65"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -2724,15 +2766,15 @@
   </mergeCells>
   <phoneticPr fontId="4"/>
   <dataValidations disablePrompts="1" count="3">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C12" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C12">
       <formula1>adjustConstValue</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C11" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C11">
       <formula1>isAbstract</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C10" xr:uid="{00000000-0002-0000-0000-000003000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C10">
       <formula1>accessScope</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -2746,20 +2788,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="8.1640625" customWidth="1"/>
-    <col min="4" max="4" width="9.83203125" customWidth="1"/>
-    <col min="6" max="6" width="13.83203125" customWidth="1"/>
+    <col min="2" max="2" width="8.125" customWidth="1"/>
+    <col min="4" max="4" width="9.875" customWidth="1"/>
+    <col min="6" max="6" width="13.875" customWidth="1"/>
     <col min="8" max="8" width="17.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="19">
+    <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>30</v>
       </c>
@@ -2775,7 +2817,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.15">
       <c r="B3" s="36" t="s">
         <v>10</v>
       </c>
@@ -2786,12 +2828,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.15">
       <c r="B4" s="37"/>
       <c r="D4" s="38"/>
       <c r="F4" s="38"/>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.15">
       <c r="B5" s="39" t="s">
         <v>11</v>
       </c>
@@ -2802,7 +2844,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.15">
       <c r="B6" s="41"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Preparing implement plain style telegram.
</commit_message>
<xml_diff>
--- a/meta/program/BlancoRestGeneratorTsConstants.xlsx
+++ b/meta/program/BlancoRestGeneratorTsConstants.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoRestGeneratorTs/meta/program/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E239B548-22A5-B946-B621-4094F8DF8C52}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F8108EE-5A2A-DD4C-89E1-05097267EB7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1000" yWindow="2700" windowWidth="21680" windowHeight="11060" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28780" yWindow="2280" windowWidth="21620" windowHeight="17540" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="constants" sheetId="1" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="178">
   <si>
     <t>定数定義書</t>
   </si>
@@ -738,6 +738,273 @@
   </si>
   <si>
     <t>"0.2.0"</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>TELEGRAM_STYLE_BLANCO</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>TELEGRAM_STYLE_PLAIN</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>"plain"</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>Task引数として渡される電文スタイル文字列: blanco</t>
+    <rPh sb="0" eb="2">
+      <t>デンブン</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>キテイ</t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>Task引数として渡される電文スタイル文字列: plain</t>
+    <rPh sb="0" eb="2">
+      <t>デンブン</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>キテイ</t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>TELEGRAM_ERROR</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>"TELEGRAM_ERROR"</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>電文種別ERRORを表す文字列</t>
+    <rPh sb="0" eb="4">
+      <t xml:space="preserve">デンブンシュベツ </t>
+    </rPh>
+    <rPh sb="10" eb="11">
+      <t xml:space="preserve">アラワス </t>
+    </rPh>
+    <rPh sb="12" eb="15">
+      <t xml:space="preserve">モジレツ </t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>TELEGRAM_TYPE_INPUT</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>"Input"</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>電文定義書に要求電文として定義された電文種別を表す文字列</t>
+    <rPh sb="0" eb="2">
+      <t xml:space="preserve">デンブｎ </t>
+    </rPh>
+    <rPh sb="2" eb="5">
+      <t xml:space="preserve">テイギショ </t>
+    </rPh>
+    <rPh sb="6" eb="8">
+      <t xml:space="preserve">ヨウキュウ </t>
+    </rPh>
+    <rPh sb="8" eb="10">
+      <t xml:space="preserve">デンブｎ </t>
+    </rPh>
+    <rPh sb="13" eb="15">
+      <t xml:space="preserve">テイギサレタ </t>
+    </rPh>
+    <rPh sb="18" eb="22">
+      <t xml:space="preserve">デンブンシュベツ </t>
+    </rPh>
+    <rPh sb="23" eb="24">
+      <t xml:space="preserve">アラワス </t>
+    </rPh>
+    <rPh sb="25" eb="28">
+      <t xml:space="preserve">モジレツ </t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>TELEGRAM_TYPE_OUTPUT</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>"Output"</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>電文定義書に応答電文として定義された電文種別を表す文字列</t>
+    <rPh sb="0" eb="2">
+      <t xml:space="preserve">デンブｎ </t>
+    </rPh>
+    <rPh sb="2" eb="5">
+      <t xml:space="preserve">テイギショ </t>
+    </rPh>
+    <rPh sb="6" eb="8">
+      <t xml:space="preserve">オウトウ </t>
+    </rPh>
+    <rPh sb="8" eb="10">
+      <t xml:space="preserve">デンブｎ </t>
+    </rPh>
+    <rPh sb="13" eb="15">
+      <t xml:space="preserve">テイギサレタ </t>
+    </rPh>
+    <rPh sb="18" eb="22">
+      <t xml:space="preserve">デンブンシュベツ </t>
+    </rPh>
+    <rPh sb="23" eb="24">
+      <t xml:space="preserve">アラワス </t>
+    </rPh>
+    <rPh sb="25" eb="28">
+      <t xml:space="preserve">モジレツ </t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>TELEGRAM_TYPE_ERROR</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>電文定義書にエラー電文として定義された電文種別を表す文字列</t>
+    <rPh sb="0" eb="2">
+      <t xml:space="preserve">デンブｎ </t>
+    </rPh>
+    <rPh sb="2" eb="5">
+      <t xml:space="preserve">テイギショ </t>
+    </rPh>
+    <rPh sb="9" eb="11">
+      <t xml:space="preserve">デンブｎ </t>
+    </rPh>
+    <rPh sb="14" eb="16">
+      <t xml:space="preserve">テイギサレタ </t>
+    </rPh>
+    <rPh sb="19" eb="23">
+      <t xml:space="preserve">デンブンシュベツ </t>
+    </rPh>
+    <rPh sb="24" eb="25">
+      <t xml:space="preserve">アラワス </t>
+    </rPh>
+    <rPh sb="26" eb="29">
+      <t xml:space="preserve">モジレツ </t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>TELEGRAM_STATUS_CODE</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>"statusCode"</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>エラー電文に追加されるstatusCodeのプロパティ名</t>
+    <rPh sb="3" eb="5">
+      <t xml:space="preserve">デンブｎ </t>
+    </rPh>
+    <rPh sb="6" eb="8">
+      <t xml:space="preserve">ツイカ </t>
+    </rPh>
+    <rPh sb="27" eb="28">
+      <t xml:space="preserve">メイ </t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>ON_CONFLICT_PREFER_PATH</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>"PREFER_PATH"</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>BODYで渡されたプロパティをURIパスで渡されたプロパティで上書きする</t>
+    <rPh sb="5" eb="6">
+      <t xml:space="preserve">ワタサレタ </t>
+    </rPh>
+    <rPh sb="21" eb="22">
+      <t xml:space="preserve">ワタサレタ </t>
+    </rPh>
+    <rPh sb="31" eb="33">
+      <t xml:space="preserve">ウワガキスル </t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>ON_CONFLICT_PREFER_BODY</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>"PREFER_BODY"</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>BODYで渡されたプロパティをURIパスより優先する</t>
+    <rPh sb="5" eb="6">
+      <t xml:space="preserve">ワタサレタ </t>
+    </rPh>
+    <rPh sb="22" eb="24">
+      <t xml:space="preserve">ユウセンスル </t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>ON_CONFLICT_REJECT</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>"REJECT"</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>BODYとURIパスでプロパティが重複した場合はREJECTする</t>
+    <rPh sb="17" eb="19">
+      <t xml:space="preserve">ジュウフク </t>
+    </rPh>
+    <rPh sb="21" eb="23">
+      <t xml:space="preserve">バアイハ </t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>TELEGRAM_QUERY_KIND_PATH</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>"path"</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>電文プロパティをQuery文字列として受け取る際の種別</t>
+    <rPh sb="0" eb="2">
+      <t xml:space="preserve">デンブｎ </t>
+    </rPh>
+    <rPh sb="13" eb="16">
+      <t xml:space="preserve">モジレツ </t>
+    </rPh>
+    <rPh sb="19" eb="20">
+      <t xml:space="preserve">ウケトル </t>
+    </rPh>
+    <rPh sb="23" eb="24">
+      <t xml:space="preserve">サイノ </t>
+    </rPh>
+    <rPh sb="25" eb="27">
+      <t xml:space="preserve">シュベツ </t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>TELEGRAM_QUERY_KIND_QUERY</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>"query"</t>
     <phoneticPr fontId="4"/>
   </si>
 </sst>
@@ -1083,29 +1350,28 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1160,7 +1426,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1169,20 +1435,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1619,10 +1884,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H65"/>
+  <dimension ref="A1:H77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="B82" sqref="B82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1705,43 +1970,43 @@
         <v>9</v>
       </c>
       <c r="D9"/>
-      <c r="E9" s="15"/>
+      <c r="E9"/>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="16" t="s">
+      <c r="A10" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="17"/>
-      <c r="C10" s="18" t="s">
+      <c r="B10" s="16"/>
+      <c r="C10" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
+      <c r="D10"/>
+      <c r="E10"/>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="16" t="s">
+      <c r="A11" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="17"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="15"/>
+      <c r="B11" s="16"/>
+      <c r="C11" s="17"/>
+      <c r="D11"/>
+      <c r="E11"/>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="16" t="s">
+      <c r="A12" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="17"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="15"/>
+      <c r="B12" s="16"/>
+      <c r="C12" s="17"/>
+      <c r="D12"/>
+      <c r="E12"/>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="15"/>
-      <c r="B13" s="15"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="15"/>
+      <c r="A13"/>
+      <c r="B13"/>
+      <c r="C13"/>
+      <c r="D13"/>
+      <c r="E13"/>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="4" t="s">
@@ -1753,13 +2018,13 @@
       <c r="E14" s="6"/>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="16" t="s">
+      <c r="A15" s="15" t="s">
         <v>15</v>
       </c>
       <c r="B15" s="7"/>
-      <c r="C15" s="19"/>
-      <c r="D15" s="20"/>
-      <c r="E15" s="21"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="20"/>
     </row>
     <row r="16" spans="1:6">
       <c r="A16"/>
@@ -1773,989 +2038,1241 @@
       <c r="A17" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="17"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
+      <c r="B17" s="16"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="16"/>
       <c r="F17" s="7"/>
       <c r="G17"/>
       <c r="H17"/>
     </row>
     <row r="18" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A18" s="43" t="s">
+      <c r="A18" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="43" t="s">
+      <c r="B18" s="41" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="44" t="s">
+      <c r="C18" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="D18" s="44" t="s">
+      <c r="D18" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="E18" s="44" t="s">
+      <c r="E18" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="F18" s="22"/>
+      <c r="F18" s="21"/>
       <c r="G18"/>
       <c r="H18"/>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" s="43"/>
-      <c r="B19" s="43"/>
-      <c r="C19" s="44"/>
-      <c r="D19" s="44"/>
-      <c r="E19" s="44"/>
-      <c r="F19" s="23"/>
+      <c r="A19" s="41"/>
+      <c r="B19" s="41"/>
+      <c r="C19" s="42"/>
+      <c r="D19" s="42"/>
+      <c r="E19" s="42"/>
+      <c r="F19" s="22"/>
       <c r="G19"/>
       <c r="H19"/>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="24">
+      <c r="A20" s="23">
         <v>1</v>
       </c>
-      <c r="B20" s="25" t="s">
+      <c r="B20" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="C20" s="26" t="s">
+      <c r="C20" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="D20" s="26" t="s">
+      <c r="D20" s="25" t="s">
         <v>114</v>
       </c>
-      <c r="E20" s="27" t="s">
+      <c r="E20" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="F20" s="28"/>
+      <c r="F20" s="27"/>
       <c r="G20"/>
       <c r="H20"/>
     </row>
     <row r="21" spans="1:8">
-      <c r="A21" s="24">
+      <c r="A21" s="23">
         <f>A20+1</f>
         <v>2</v>
       </c>
-      <c r="B21" s="25" t="s">
+      <c r="B21" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="C21" s="26" t="s">
+      <c r="C21" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="D21" s="26" t="s">
+      <c r="D21" s="25" t="s">
         <v>115</v>
       </c>
-      <c r="E21" s="29" t="s">
+      <c r="E21" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="F21" s="30"/>
+      <c r="F21" s="29"/>
       <c r="G21"/>
       <c r="H21"/>
     </row>
     <row r="22" spans="1:8">
-      <c r="A22" s="24">
-        <f>A21+1</f>
+      <c r="A22" s="23">
+        <f t="shared" ref="A22:A76" si="0">A21+1</f>
         <v>3</v>
       </c>
-      <c r="B22" s="25" t="s">
+      <c r="B22" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="C22" s="26" t="s">
+      <c r="C22" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="D22" s="26" t="s">
+      <c r="D22" s="25" t="s">
         <v>144</v>
       </c>
-      <c r="E22" s="26" t="s">
+      <c r="E22" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="F22" s="30"/>
+      <c r="F22" s="29"/>
       <c r="G22"/>
       <c r="H22"/>
     </row>
     <row r="23" spans="1:8">
-      <c r="A23" s="24">
-        <f t="shared" ref="A23:A64" si="0">A22+1</f>
+      <c r="A23" s="23">
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B23" s="25" t="s">
+      <c r="B23" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="C23" s="26" t="s">
+      <c r="C23" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="D23" s="26" t="s">
+      <c r="D23" s="25" t="s">
         <v>116</v>
       </c>
-      <c r="E23" s="26" t="s">
+      <c r="E23" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="F23" s="30"/>
+      <c r="F23" s="29"/>
       <c r="G23"/>
       <c r="H23"/>
     </row>
     <row r="24" spans="1:8">
-      <c r="A24" s="24">
+      <c r="A24" s="23">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B24" s="25" t="s">
+      <c r="B24" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="C24" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="D24" s="26" t="s">
+      <c r="C24" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="D24" s="25" t="s">
         <v>117</v>
       </c>
-      <c r="E24" s="26" t="s">
+      <c r="E24" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="F24" s="30"/>
+      <c r="F24" s="29"/>
       <c r="G24"/>
       <c r="H24"/>
     </row>
-    <row r="25" spans="1:8" s="42" customFormat="1">
-      <c r="A25" s="24">
+    <row r="25" spans="1:8">
+      <c r="A25" s="23">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B25" s="25" t="s">
+      <c r="B25" s="24" t="s">
         <v>100</v>
       </c>
-      <c r="C25" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="D25" s="26" t="s">
+      <c r="C25" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="D25" s="25" t="s">
         <v>101</v>
       </c>
-      <c r="E25" s="26" t="s">
+      <c r="E25" s="25" t="s">
         <v>102</v>
       </c>
-      <c r="F25" s="30"/>
+      <c r="F25" s="29"/>
       <c r="G25"/>
       <c r="H25"/>
     </row>
-    <row r="26" spans="1:8" s="42" customFormat="1">
-      <c r="A26" s="24">
+    <row r="26" spans="1:8">
+      <c r="A26" s="23">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B26" s="25" t="s">
+      <c r="B26" s="24" t="s">
         <v>103</v>
       </c>
-      <c r="C26" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="D26" s="26" t="s">
+      <c r="C26" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="D26" s="25" t="s">
         <v>104</v>
       </c>
-      <c r="E26" s="26" t="s">
+      <c r="E26" s="25" t="s">
         <v>102</v>
       </c>
-      <c r="F26" s="30"/>
+      <c r="F26" s="29"/>
       <c r="G26"/>
       <c r="H26"/>
     </row>
-    <row r="27" spans="1:8" s="42" customFormat="1">
-      <c r="A27" s="24">
+    <row r="27" spans="1:8">
+      <c r="A27" s="23">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B27" s="25" t="s">
+      <c r="B27" s="24" t="s">
         <v>105</v>
       </c>
-      <c r="C27" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="D27" s="26" t="s">
+      <c r="C27" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="D27" s="25" t="s">
         <v>106</v>
       </c>
-      <c r="E27" s="26" t="s">
+      <c r="E27" s="25" t="s">
         <v>102</v>
       </c>
-      <c r="F27" s="30"/>
+      <c r="F27" s="29"/>
       <c r="G27"/>
       <c r="H27"/>
     </row>
-    <row r="28" spans="1:8" s="42" customFormat="1">
-      <c r="A28" s="24">
+    <row r="28" spans="1:8">
+      <c r="A28" s="23">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B28" s="25" t="s">
+      <c r="B28" s="24" t="s">
         <v>107</v>
       </c>
-      <c r="C28" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="D28" s="26" t="s">
+      <c r="C28" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="D28" s="25" t="s">
         <v>108</v>
       </c>
-      <c r="E28" s="26" t="s">
+      <c r="E28" s="25" t="s">
         <v>109</v>
       </c>
-      <c r="F28" s="30"/>
+      <c r="F28" s="29"/>
       <c r="G28"/>
       <c r="H28"/>
     </row>
-    <row r="29" spans="1:8" s="42" customFormat="1">
-      <c r="A29" s="24">
+    <row r="29" spans="1:8">
+      <c r="A29" s="23">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B29" s="25" t="s">
+      <c r="B29" s="24" t="s">
         <v>110</v>
       </c>
-      <c r="C29" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="D29" s="26" t="s">
+      <c r="C29" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="D29" s="25" t="s">
         <v>120</v>
       </c>
-      <c r="E29" s="26" t="s">
+      <c r="E29" s="25" t="s">
         <v>109</v>
       </c>
-      <c r="F29" s="32"/>
+      <c r="F29" s="31"/>
       <c r="G29"/>
       <c r="H29"/>
     </row>
     <row r="30" spans="1:8">
-      <c r="A30" s="24">
+      <c r="A30" s="23">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="B30" s="25" t="s">
+      <c r="B30" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="C30" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="D30" s="26" t="s">
+      <c r="C30" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="D30" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="E30" s="26" t="s">
+      <c r="E30" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="F30" s="30"/>
+      <c r="F30" s="29"/>
       <c r="G30"/>
       <c r="H30"/>
     </row>
     <row r="31" spans="1:8">
-      <c r="A31" s="24">
+      <c r="A31" s="23">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="B31" s="25" t="s">
+      <c r="B31" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="C31" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="D31" s="26" t="s">
+      <c r="C31" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="D31" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="E31" s="26" t="s">
+      <c r="E31" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="F31" s="30"/>
+      <c r="F31" s="29"/>
       <c r="G31"/>
       <c r="H31"/>
     </row>
     <row r="32" spans="1:8">
-      <c r="A32" s="24">
+      <c r="A32" s="23">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="B32" s="25" t="s">
+      <c r="B32" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="C32" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="D32" s="26" t="s">
+      <c r="C32" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="D32" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="E32" s="26" t="s">
+      <c r="E32" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="F32" s="30"/>
+      <c r="F32" s="29"/>
       <c r="G32"/>
       <c r="H32"/>
     </row>
     <row r="33" spans="1:8">
-      <c r="A33" s="24">
+      <c r="A33" s="23">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="B33" s="25" t="s">
+      <c r="B33" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="C33" s="31" t="s">
-        <v>33</v>
-      </c>
-      <c r="D33" s="31" t="s">
+      <c r="C33" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="D33" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="E33" s="31" t="s">
+      <c r="E33" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="F33" s="32"/>
+      <c r="F33" s="31"/>
       <c r="G33"/>
       <c r="H33"/>
     </row>
     <row r="34" spans="1:8">
-      <c r="A34" s="24">
+      <c r="A34" s="23">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="B34" s="25" t="s">
+      <c r="B34" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="C34" s="31" t="s">
-        <v>33</v>
-      </c>
-      <c r="D34" s="31" t="s">
+      <c r="C34" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="D34" s="30" t="s">
         <v>47</v>
       </c>
-      <c r="E34" s="31" t="s">
+      <c r="E34" s="30" t="s">
         <v>48</v>
       </c>
-      <c r="F34" s="32"/>
+      <c r="F34" s="31"/>
       <c r="G34"/>
       <c r="H34"/>
     </row>
     <row r="35" spans="1:8">
-      <c r="A35" s="24">
+      <c r="A35" s="23">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="B35" s="25" t="s">
+      <c r="B35" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="C35" s="31" t="s">
-        <v>33</v>
-      </c>
-      <c r="D35" s="31" t="s">
+      <c r="C35" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="D35" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="E35" s="31" t="s">
+      <c r="E35" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="F35" s="32"/>
+      <c r="F35" s="31"/>
       <c r="G35"/>
       <c r="H35"/>
     </row>
     <row r="36" spans="1:8">
-      <c r="A36" s="24">
+      <c r="A36" s="23">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="B36" s="25" t="s">
+      <c r="B36" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="C36" s="31" t="s">
-        <v>33</v>
-      </c>
-      <c r="D36" s="31" t="s">
+      <c r="C36" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="D36" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="E36" s="31" t="s">
+      <c r="E36" s="30" t="s">
         <v>52</v>
       </c>
-      <c r="F36" s="32"/>
+      <c r="F36" s="31"/>
       <c r="G36"/>
       <c r="H36"/>
     </row>
     <row r="37" spans="1:8">
-      <c r="A37" s="24">
+      <c r="A37" s="23">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="B37" s="25" t="s">
+      <c r="B37" s="24" t="s">
         <v>64</v>
       </c>
-      <c r="C37" s="31" t="s">
-        <v>33</v>
-      </c>
-      <c r="D37" s="31" t="s">
+      <c r="C37" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="D37" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="E37" s="31" t="s">
+      <c r="E37" s="30" t="s">
         <v>52</v>
       </c>
-      <c r="F37" s="32"/>
+      <c r="F37" s="31"/>
       <c r="G37"/>
       <c r="H37"/>
     </row>
     <row r="38" spans="1:8">
-      <c r="A38" s="24">
+      <c r="A38" s="23">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="B38" s="25" t="s">
+      <c r="B38" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="C38" s="31" t="s">
-        <v>33</v>
-      </c>
-      <c r="D38" s="31" t="s">
+      <c r="C38" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="D38" s="30" t="s">
         <v>57</v>
       </c>
-      <c r="E38" s="31" t="s">
+      <c r="E38" s="30" t="s">
         <v>52</v>
       </c>
-      <c r="F38" s="32"/>
+      <c r="F38" s="31"/>
       <c r="G38"/>
       <c r="H38"/>
     </row>
     <row r="39" spans="1:8">
-      <c r="A39" s="24">
+      <c r="A39" s="23">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="B39" s="25" t="s">
+      <c r="B39" s="24" t="s">
         <v>66</v>
       </c>
-      <c r="C39" s="31" t="s">
-        <v>33</v>
-      </c>
-      <c r="D39" s="31" t="s">
+      <c r="C39" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="D39" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="E39" s="31" t="s">
+      <c r="E39" s="30" t="s">
         <v>52</v>
       </c>
-      <c r="F39" s="32"/>
+      <c r="F39" s="31"/>
       <c r="G39"/>
       <c r="H39"/>
     </row>
     <row r="40" spans="1:8">
-      <c r="A40" s="24">
+      <c r="A40" s="23">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="B40" s="33" t="s">
+      <c r="B40" s="32" t="s">
         <v>67</v>
       </c>
-      <c r="C40" s="34" t="s">
-        <v>33</v>
-      </c>
-      <c r="D40" s="34" t="s">
+      <c r="C40" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="D40" s="33" t="s">
         <v>59</v>
       </c>
-      <c r="E40" s="34" t="s">
+      <c r="E40" s="33" t="s">
         <v>53</v>
       </c>
-      <c r="F40" s="35"/>
+      <c r="F40" s="34"/>
       <c r="G40"/>
       <c r="H40"/>
     </row>
     <row r="41" spans="1:8">
-      <c r="A41" s="24">
+      <c r="A41" s="23">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="B41" s="33" t="s">
+      <c r="B41" s="32" t="s">
         <v>68</v>
       </c>
-      <c r="C41" s="34" t="s">
-        <v>33</v>
-      </c>
-      <c r="D41" s="34" t="s">
+      <c r="C41" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="D41" s="33" t="s">
         <v>62</v>
       </c>
-      <c r="E41" s="34" t="s">
+      <c r="E41" s="33" t="s">
         <v>53</v>
       </c>
-      <c r="F41" s="35"/>
+      <c r="F41" s="34"/>
       <c r="G41"/>
       <c r="H41"/>
     </row>
     <row r="42" spans="1:8">
-      <c r="A42" s="24">
+      <c r="A42" s="23">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="B42" s="33" t="s">
+      <c r="B42" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="C42" s="34" t="s">
-        <v>33</v>
-      </c>
-      <c r="D42" s="34" t="s">
+      <c r="C42" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="D42" s="33" t="s">
         <v>60</v>
       </c>
-      <c r="E42" s="34" t="s">
+      <c r="E42" s="33" t="s">
         <v>53</v>
       </c>
-      <c r="F42" s="35"/>
+      <c r="F42" s="34"/>
       <c r="G42"/>
       <c r="H42"/>
     </row>
     <row r="43" spans="1:8">
-      <c r="A43" s="24">
+      <c r="A43" s="23">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="B43" s="33" t="s">
+      <c r="B43" s="32" t="s">
         <v>70</v>
       </c>
-      <c r="C43" s="34" t="s">
-        <v>33</v>
-      </c>
-      <c r="D43" s="34" t="s">
+      <c r="C43" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="D43" s="33" t="s">
         <v>61</v>
       </c>
-      <c r="E43" s="34" t="s">
+      <c r="E43" s="33" t="s">
         <v>53</v>
       </c>
-      <c r="F43" s="35"/>
+      <c r="F43" s="34"/>
       <c r="G43"/>
       <c r="H43"/>
     </row>
     <row r="44" spans="1:8">
-      <c r="A44" s="24">
+      <c r="A44" s="23">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="B44" s="33" t="s">
+      <c r="B44" s="32" t="s">
         <v>71</v>
       </c>
-      <c r="C44" s="34" t="s">
-        <v>33</v>
-      </c>
-      <c r="D44" s="34" t="s">
+      <c r="C44" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="D44" s="33" t="s">
         <v>118</v>
       </c>
-      <c r="E44" s="34" t="s">
+      <c r="E44" s="33" t="s">
         <v>72</v>
       </c>
-      <c r="F44" s="35"/>
+      <c r="F44" s="34"/>
       <c r="G44"/>
       <c r="H44"/>
     </row>
     <row r="45" spans="1:8">
-      <c r="A45" s="24">
+      <c r="A45" s="23">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="B45" s="33" t="s">
+      <c r="B45" s="32" t="s">
         <v>73</v>
       </c>
-      <c r="C45" s="34" t="s">
-        <v>33</v>
-      </c>
-      <c r="D45" s="34" t="s">
+      <c r="C45" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="D45" s="33" t="s">
         <v>119</v>
       </c>
-      <c r="E45" s="34" t="s">
+      <c r="E45" s="33" t="s">
         <v>74</v>
       </c>
-      <c r="F45" s="35"/>
+      <c r="F45" s="34"/>
       <c r="G45"/>
       <c r="H45"/>
     </row>
     <row r="46" spans="1:8">
-      <c r="A46" s="24">
+      <c r="A46" s="23">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="B46" s="33" t="s">
+      <c r="B46" s="32" t="s">
         <v>77</v>
       </c>
-      <c r="C46" s="34" t="s">
-        <v>33</v>
-      </c>
-      <c r="D46" s="34" t="s">
+      <c r="C46" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="D46" s="33" t="s">
         <v>75</v>
       </c>
-      <c r="E46" s="34" t="s">
+      <c r="E46" s="33" t="s">
         <v>76</v>
       </c>
-      <c r="F46" s="35"/>
+      <c r="F46" s="34"/>
     </row>
     <row r="47" spans="1:8">
-      <c r="A47" s="24">
+      <c r="A47" s="23">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="B47" s="33" t="s">
+      <c r="B47" s="32" t="s">
         <v>78</v>
       </c>
-      <c r="C47" s="34" t="s">
-        <v>33</v>
-      </c>
-      <c r="D47" s="34" t="s">
+      <c r="C47" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="D47" s="33" t="s">
         <v>139</v>
       </c>
-      <c r="E47" s="34" t="s">
+      <c r="E47" s="33" t="s">
         <v>79</v>
       </c>
-      <c r="F47" s="35"/>
+      <c r="F47" s="34"/>
     </row>
     <row r="48" spans="1:8">
-      <c r="A48" s="24">
+      <c r="A48" s="23">
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-      <c r="B48" s="33" t="s">
+      <c r="B48" s="32" t="s">
         <v>82</v>
       </c>
-      <c r="C48" s="34" t="s">
-        <v>33</v>
-      </c>
-      <c r="D48" s="34" t="s">
+      <c r="C48" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="D48" s="33" t="s">
         <v>99</v>
       </c>
-      <c r="E48" s="34" t="s">
+      <c r="E48" s="33" t="s">
         <v>80</v>
       </c>
-      <c r="F48" s="35"/>
+      <c r="F48" s="34"/>
     </row>
     <row r="49" spans="1:8">
-      <c r="A49" s="24">
+      <c r="A49" s="23">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="B49" s="33" t="s">
+      <c r="B49" s="32" t="s">
         <v>81</v>
       </c>
-      <c r="C49" s="34" t="s">
-        <v>33</v>
-      </c>
-      <c r="D49" s="34" t="s">
+      <c r="C49" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="D49" s="33" t="s">
         <v>83</v>
       </c>
-      <c r="E49" s="34" t="s">
+      <c r="E49" s="33" t="s">
         <v>84</v>
       </c>
-      <c r="F49" s="35"/>
+      <c r="F49" s="34"/>
     </row>
     <row r="50" spans="1:8">
-      <c r="A50" s="24">
+      <c r="A50" s="23">
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="B50" s="25" t="s">
+      <c r="B50" s="24" t="s">
         <v>85</v>
       </c>
-      <c r="C50" s="31" t="s">
-        <v>33</v>
-      </c>
-      <c r="D50" s="31" t="s">
+      <c r="C50" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="D50" s="30" t="s">
         <v>93</v>
       </c>
-      <c r="E50" s="31" t="s">
+      <c r="E50" s="30" t="s">
         <v>98</v>
       </c>
-      <c r="F50" s="32"/>
+      <c r="F50" s="31"/>
       <c r="G50"/>
       <c r="H50"/>
     </row>
     <row r="51" spans="1:8">
-      <c r="A51" s="24">
+      <c r="A51" s="23">
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="B51" s="25" t="s">
+      <c r="B51" s="24" t="s">
         <v>86</v>
       </c>
-      <c r="C51" s="31" t="s">
-        <v>33</v>
-      </c>
-      <c r="D51" s="31" t="s">
+      <c r="C51" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="D51" s="30" t="s">
         <v>94</v>
       </c>
-      <c r="E51" s="31" t="s">
+      <c r="E51" s="30" t="s">
         <v>97</v>
       </c>
-      <c r="F51" s="32"/>
+      <c r="F51" s="31"/>
       <c r="G51"/>
       <c r="H51"/>
     </row>
     <row r="52" spans="1:8">
-      <c r="A52" s="24">
-        <f t="shared" si="0"/>
-        <v>33</v>
-      </c>
-      <c r="B52" s="25" t="s">
+      <c r="A52" s="23">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="B52" s="24" t="s">
         <v>87</v>
       </c>
-      <c r="C52" s="31" t="s">
-        <v>33</v>
-      </c>
-      <c r="D52" s="31" t="s">
+      <c r="C52" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="D52" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="E52" s="31" t="s">
+      <c r="E52" s="30" t="s">
         <v>97</v>
       </c>
-      <c r="F52" s="32"/>
+      <c r="F52" s="31"/>
       <c r="G52"/>
       <c r="H52"/>
     </row>
     <row r="53" spans="1:8">
-      <c r="A53" s="24">
+      <c r="A53" s="23">
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
-      <c r="B53" s="25" t="s">
+      <c r="B53" s="24" t="s">
         <v>88</v>
       </c>
-      <c r="C53" s="31" t="s">
-        <v>33</v>
-      </c>
-      <c r="D53" s="31" t="s">
+      <c r="C53" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="D53" s="30" t="s">
         <v>96</v>
       </c>
-      <c r="E53" s="31" t="s">
+      <c r="E53" s="30" t="s">
         <v>97</v>
       </c>
-      <c r="F53" s="32"/>
+      <c r="F53" s="31"/>
       <c r="G53"/>
       <c r="H53"/>
     </row>
     <row r="54" spans="1:8">
-      <c r="A54" s="24">
+      <c r="A54" s="23">
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
-      <c r="B54" s="33" t="s">
+      <c r="B54" s="32" t="s">
         <v>89</v>
       </c>
-      <c r="C54" s="34" t="s">
-        <v>33</v>
-      </c>
-      <c r="D54" s="34" t="s">
+      <c r="C54" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="D54" s="33" t="s">
         <v>93</v>
       </c>
-      <c r="E54" s="34" t="s">
+      <c r="E54" s="33" t="s">
         <v>97</v>
       </c>
-      <c r="F54" s="35"/>
+      <c r="F54" s="34"/>
       <c r="G54"/>
       <c r="H54"/>
     </row>
     <row r="55" spans="1:8">
-      <c r="A55" s="24">
+      <c r="A55" s="23">
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
-      <c r="B55" s="33" t="s">
+      <c r="B55" s="32" t="s">
         <v>90</v>
       </c>
-      <c r="C55" s="34" t="s">
-        <v>33</v>
-      </c>
-      <c r="D55" s="34" t="s">
+      <c r="C55" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="D55" s="33" t="s">
         <v>94</v>
       </c>
-      <c r="E55" s="34" t="s">
+      <c r="E55" s="33" t="s">
         <v>97</v>
       </c>
-      <c r="F55" s="35"/>
+      <c r="F55" s="34"/>
       <c r="G55"/>
       <c r="H55"/>
     </row>
     <row r="56" spans="1:8">
-      <c r="A56" s="24">
+      <c r="A56" s="23">
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="B56" s="33" t="s">
+      <c r="B56" s="32" t="s">
         <v>91</v>
       </c>
-      <c r="C56" s="34" t="s">
-        <v>33</v>
-      </c>
-      <c r="D56" s="34" t="s">
+      <c r="C56" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="D56" s="33" t="s">
         <v>95</v>
       </c>
-      <c r="E56" s="34" t="s">
+      <c r="E56" s="33" t="s">
         <v>97</v>
       </c>
-      <c r="F56" s="35"/>
+      <c r="F56" s="34"/>
       <c r="G56"/>
       <c r="H56"/>
     </row>
     <row r="57" spans="1:8">
-      <c r="A57" s="24">
+      <c r="A57" s="23">
         <f t="shared" si="0"/>
         <v>38</v>
       </c>
-      <c r="B57" s="33" t="s">
+      <c r="B57" s="32" t="s">
         <v>92</v>
       </c>
-      <c r="C57" s="34" t="s">
-        <v>33</v>
-      </c>
-      <c r="D57" s="34" t="s">
+      <c r="C57" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="D57" s="33" t="s">
         <v>96</v>
       </c>
-      <c r="E57" s="34" t="s">
+      <c r="E57" s="33" t="s">
         <v>97</v>
       </c>
-      <c r="F57" s="35"/>
+      <c r="F57" s="34"/>
       <c r="G57"/>
       <c r="H57"/>
     </row>
     <row r="58" spans="1:8">
-      <c r="A58" s="24">
+      <c r="A58" s="23">
         <f t="shared" si="0"/>
         <v>39</v>
       </c>
-      <c r="B58" s="33" t="s">
+      <c r="B58" s="32" t="s">
         <v>121</v>
       </c>
-      <c r="C58" s="34" t="s">
-        <v>33</v>
-      </c>
-      <c r="D58" s="34" t="s">
+      <c r="C58" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="D58" s="33" t="s">
         <v>127</v>
       </c>
-      <c r="E58" s="34" t="s">
+      <c r="E58" s="33" t="s">
         <v>133</v>
       </c>
-      <c r="F58" s="35"/>
+      <c r="F58" s="34"/>
       <c r="G58"/>
       <c r="H58"/>
     </row>
     <row r="59" spans="1:8">
-      <c r="A59" s="24">
+      <c r="A59" s="23">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="B59" s="33" t="s">
+      <c r="B59" s="32" t="s">
         <v>122</v>
       </c>
-      <c r="C59" s="34" t="s">
-        <v>33</v>
-      </c>
-      <c r="D59" s="34" t="s">
+      <c r="C59" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="D59" s="33" t="s">
         <v>128</v>
       </c>
-      <c r="E59" s="34" t="s">
+      <c r="E59" s="33" t="s">
         <v>134</v>
       </c>
-      <c r="F59" s="35"/>
+      <c r="F59" s="34"/>
       <c r="G59"/>
       <c r="H59"/>
     </row>
     <row r="60" spans="1:8">
-      <c r="A60" s="24">
+      <c r="A60" s="23">
         <f t="shared" si="0"/>
         <v>41</v>
       </c>
-      <c r="B60" s="33" t="s">
+      <c r="B60" s="32" t="s">
         <v>123</v>
       </c>
-      <c r="C60" s="34" t="s">
+      <c r="C60" s="33" t="s">
         <v>140</v>
       </c>
-      <c r="D60" s="34" t="s">
+      <c r="D60" s="33" t="s">
         <v>129</v>
       </c>
-      <c r="E60" s="34" t="s">
+      <c r="E60" s="33" t="s">
         <v>135</v>
       </c>
-      <c r="F60" s="35"/>
+      <c r="F60" s="34"/>
       <c r="G60"/>
       <c r="H60"/>
     </row>
     <row r="61" spans="1:8">
-      <c r="A61" s="24">
+      <c r="A61" s="23">
         <f t="shared" si="0"/>
         <v>42</v>
       </c>
-      <c r="B61" s="33" t="s">
+      <c r="B61" s="32" t="s">
         <v>124</v>
       </c>
-      <c r="C61" s="34" t="s">
-        <v>33</v>
-      </c>
-      <c r="D61" s="34" t="s">
+      <c r="C61" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="D61" s="33" t="s">
         <v>130</v>
       </c>
-      <c r="E61" s="34" t="s">
+      <c r="E61" s="33" t="s">
         <v>136</v>
       </c>
-      <c r="F61" s="35"/>
+      <c r="F61" s="34"/>
       <c r="G61"/>
       <c r="H61"/>
     </row>
     <row r="62" spans="1:8">
-      <c r="A62" s="24">
+      <c r="A62" s="23">
         <f t="shared" si="0"/>
         <v>43</v>
       </c>
-      <c r="B62" s="33" t="s">
+      <c r="B62" s="32" t="s">
         <v>125</v>
       </c>
-      <c r="C62" s="34" t="s">
-        <v>33</v>
-      </c>
-      <c r="D62" s="34" t="s">
+      <c r="C62" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="D62" s="33" t="s">
         <v>131</v>
       </c>
-      <c r="E62" s="34" t="s">
+      <c r="E62" s="33" t="s">
         <v>137</v>
       </c>
-      <c r="F62" s="35"/>
+      <c r="F62" s="34"/>
       <c r="G62"/>
       <c r="H62"/>
     </row>
     <row r="63" spans="1:8">
-      <c r="A63" s="24">
+      <c r="A63" s="23">
         <f t="shared" si="0"/>
         <v>44</v>
       </c>
-      <c r="B63" s="33" t="s">
+      <c r="B63" s="32" t="s">
         <v>126</v>
       </c>
-      <c r="C63" s="34" t="s">
-        <v>33</v>
-      </c>
-      <c r="D63" s="34" t="s">
+      <c r="C63" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="D63" s="33" t="s">
         <v>132</v>
       </c>
-      <c r="E63" s="34" t="s">
+      <c r="E63" s="33" t="s">
         <v>138</v>
       </c>
-      <c r="F63" s="35"/>
+      <c r="F63" s="34"/>
       <c r="G63"/>
       <c r="H63"/>
     </row>
     <row r="64" spans="1:8">
-      <c r="A64" s="24">
+      <c r="A64" s="23">
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
-      <c r="B64" s="33" t="s">
-        <v>141</v>
-      </c>
-      <c r="C64" s="34" t="s">
-        <v>33</v>
-      </c>
-      <c r="D64" s="34" t="s">
-        <v>142</v>
-      </c>
-      <c r="E64" s="34" t="s">
-        <v>143</v>
-      </c>
-      <c r="F64" s="35"/>
+      <c r="B64" s="32" t="s">
+        <v>150</v>
+      </c>
+      <c r="C64" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="D64" s="33" t="s">
+        <v>151</v>
+      </c>
+      <c r="E64" s="33" t="s">
+        <v>152</v>
+      </c>
+      <c r="F64" s="34"/>
       <c r="G64"/>
       <c r="H64"/>
     </row>
     <row r="65" spans="1:8">
-      <c r="A65" s="24"/>
-      <c r="B65" s="33"/>
-      <c r="C65" s="34"/>
-      <c r="D65" s="34"/>
-      <c r="E65" s="34"/>
-      <c r="F65" s="35"/>
+      <c r="A65" s="23">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="B65" s="32" t="s">
+        <v>141</v>
+      </c>
+      <c r="C65" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="D65" s="33" t="s">
+        <v>142</v>
+      </c>
+      <c r="E65" s="33" t="s">
+        <v>143</v>
+      </c>
+      <c r="F65" s="34"/>
       <c r="G65"/>
       <c r="H65"/>
+    </row>
+    <row r="66" spans="1:8">
+      <c r="A66" s="23">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="B66" s="24" t="s">
+        <v>153</v>
+      </c>
+      <c r="C66" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="D66" s="25" t="s">
+        <v>154</v>
+      </c>
+      <c r="E66" s="25" t="s">
+        <v>155</v>
+      </c>
+      <c r="F66" s="29"/>
+      <c r="G66"/>
+      <c r="H66"/>
+    </row>
+    <row r="67" spans="1:8">
+      <c r="A67" s="23">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="B67" s="24" t="s">
+        <v>156</v>
+      </c>
+      <c r="C67" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="D67" s="25" t="s">
+        <v>157</v>
+      </c>
+      <c r="E67" s="25" t="s">
+        <v>158</v>
+      </c>
+      <c r="F67" s="29"/>
+      <c r="G67"/>
+      <c r="H67"/>
+    </row>
+    <row r="68" spans="1:8">
+      <c r="A68" s="23">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+      <c r="B68" s="24" t="s">
+        <v>159</v>
+      </c>
+      <c r="C68" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="D68" s="25" t="s">
+        <v>139</v>
+      </c>
+      <c r="E68" s="25" t="s">
+        <v>160</v>
+      </c>
+      <c r="F68" s="29"/>
+      <c r="G68"/>
+      <c r="H68"/>
+    </row>
+    <row r="69" spans="1:8">
+      <c r="A69" s="23">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="B69" s="32" t="s">
+        <v>145</v>
+      </c>
+      <c r="C69" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="D69" s="33" t="s">
+        <v>101</v>
+      </c>
+      <c r="E69" s="33" t="s">
+        <v>148</v>
+      </c>
+      <c r="F69" s="34"/>
+      <c r="G69"/>
+      <c r="H69"/>
+    </row>
+    <row r="70" spans="1:8">
+      <c r="A70" s="23">
+        <f t="shared" si="0"/>
+        <v>51</v>
+      </c>
+      <c r="B70" s="32" t="s">
+        <v>146</v>
+      </c>
+      <c r="C70" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="D70" s="33" t="s">
+        <v>147</v>
+      </c>
+      <c r="E70" s="33" t="s">
+        <v>149</v>
+      </c>
+      <c r="F70" s="34"/>
+      <c r="G70"/>
+      <c r="H70"/>
+    </row>
+    <row r="71" spans="1:8">
+      <c r="A71" s="23">
+        <f t="shared" si="0"/>
+        <v>52</v>
+      </c>
+      <c r="B71" s="24" t="s">
+        <v>161</v>
+      </c>
+      <c r="C71" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="D71" s="25" t="s">
+        <v>162</v>
+      </c>
+      <c r="E71" s="25" t="s">
+        <v>163</v>
+      </c>
+      <c r="F71" s="29"/>
+      <c r="G71"/>
+      <c r="H71"/>
+    </row>
+    <row r="72" spans="1:8">
+      <c r="A72" s="23">
+        <f t="shared" si="0"/>
+        <v>53</v>
+      </c>
+      <c r="B72" s="24" t="s">
+        <v>164</v>
+      </c>
+      <c r="C72" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="D72" s="25" t="s">
+        <v>165</v>
+      </c>
+      <c r="E72" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="F72" s="29"/>
+      <c r="G72"/>
+      <c r="H72"/>
+    </row>
+    <row r="73" spans="1:8">
+      <c r="A73" s="23">
+        <f t="shared" si="0"/>
+        <v>54</v>
+      </c>
+      <c r="B73" s="24" t="s">
+        <v>167</v>
+      </c>
+      <c r="C73" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="D73" s="25" t="s">
+        <v>168</v>
+      </c>
+      <c r="E73" s="25" t="s">
+        <v>169</v>
+      </c>
+      <c r="F73" s="29"/>
+      <c r="G73"/>
+      <c r="H73"/>
+    </row>
+    <row r="74" spans="1:8">
+      <c r="A74" s="23">
+        <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
+      <c r="B74" s="24" t="s">
+        <v>170</v>
+      </c>
+      <c r="C74" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="D74" s="25" t="s">
+        <v>171</v>
+      </c>
+      <c r="E74" s="25" t="s">
+        <v>172</v>
+      </c>
+      <c r="F74" s="29"/>
+      <c r="G74"/>
+      <c r="H74"/>
+    </row>
+    <row r="75" spans="1:8">
+      <c r="A75" s="23">
+        <f t="shared" si="0"/>
+        <v>56</v>
+      </c>
+      <c r="B75" s="24" t="s">
+        <v>173</v>
+      </c>
+      <c r="C75" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="D75" s="25" t="s">
+        <v>174</v>
+      </c>
+      <c r="E75" s="25" t="s">
+        <v>175</v>
+      </c>
+      <c r="F75" s="29"/>
+      <c r="G75"/>
+      <c r="H75"/>
+    </row>
+    <row r="76" spans="1:8">
+      <c r="A76" s="23">
+        <f t="shared" si="0"/>
+        <v>57</v>
+      </c>
+      <c r="B76" s="24" t="s">
+        <v>176</v>
+      </c>
+      <c r="C76" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="D76" s="25" t="s">
+        <v>177</v>
+      </c>
+      <c r="E76" s="25" t="s">
+        <v>175</v>
+      </c>
+      <c r="F76" s="29"/>
+      <c r="G76"/>
+      <c r="H76"/>
+    </row>
+    <row r="77" spans="1:8">
+      <c r="A77" s="23"/>
+      <c r="B77" s="32"/>
+      <c r="C77" s="33"/>
+      <c r="D77" s="33"/>
+      <c r="E77" s="33"/>
+      <c r="F77" s="34"/>
+      <c r="G77"/>
+      <c r="H77"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -2819,34 +3336,34 @@
       </c>
     </row>
     <row r="3" spans="1:10">
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="36" t="s">
+      <c r="D3" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="36" t="s">
+      <c r="F3" s="35" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:10">
-      <c r="B4" s="37"/>
-      <c r="D4" s="38"/>
-      <c r="F4" s="38"/>
+      <c r="B4" s="36"/>
+      <c r="D4" s="37"/>
+      <c r="F4" s="37"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="B5" s="39" t="s">
+      <c r="B5" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="40" t="s">
+      <c r="D5" s="39" t="s">
         <v>31</v>
       </c>
-      <c r="F5" s="40" t="s">
+      <c r="F5" s="39" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="B6" s="41"/>
+      <c r="B6" s="40"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4"/>

</xml_diff>

<commit_message>
3.1.10 Implement strictNullable option. Default false. on true, depend " | undefined | null" to type of nullable properties.
</commit_message>
<xml_diff>
--- a/meta/program/BlancoRestGeneratorTsConstants.xlsx
+++ b/meta/program/BlancoRestGeneratorTsConstants.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoRestGeneratorTs/meta/program/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EF71B88-40EC-D849-8E9C-400F5A55949A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{033492F4-E162-4444-8785-E064F1055D7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28780" yWindow="2280" windowWidth="21620" windowHeight="17540" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -737,10 +737,6 @@
     <phoneticPr fontId="4"/>
   </si>
   <si>
-    <t>"0.2.0"</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
     <t>TELEGRAM_STYLE_BLANCO</t>
     <phoneticPr fontId="4"/>
   </si>
@@ -1050,6 +1046,10 @@
   </si>
   <si>
     <t>"DELETE"</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>"3.1.10"</t>
     <phoneticPr fontId="4"/>
   </si>
 </sst>
@@ -1931,8 +1931,8 @@
   </sheetPr>
   <dimension ref="A1:H81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="D82" sqref="D82"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -2174,7 +2174,7 @@
         <v>22</v>
       </c>
       <c r="D22" s="25" t="s">
-        <v>144</v>
+        <v>186</v>
       </c>
       <c r="E22" s="25" t="s">
         <v>27</v>
@@ -3042,16 +3042,16 @@
         <v>45</v>
       </c>
       <c r="B64" s="32" t="s">
+        <v>149</v>
+      </c>
+      <c r="C64" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="D64" s="33" t="s">
         <v>150</v>
       </c>
-      <c r="C64" s="33" t="s">
-        <v>33</v>
-      </c>
-      <c r="D64" s="33" t="s">
+      <c r="E64" s="33" t="s">
         <v>151</v>
-      </c>
-      <c r="E64" s="33" t="s">
-        <v>152</v>
       </c>
       <c r="F64" s="34"/>
       <c r="G64"/>
@@ -3084,16 +3084,16 @@
         <v>47</v>
       </c>
       <c r="B66" s="24" t="s">
+        <v>152</v>
+      </c>
+      <c r="C66" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="D66" s="25" t="s">
         <v>153</v>
       </c>
-      <c r="C66" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="D66" s="25" t="s">
+      <c r="E66" s="25" t="s">
         <v>154</v>
-      </c>
-      <c r="E66" s="25" t="s">
-        <v>155</v>
       </c>
       <c r="F66" s="29"/>
       <c r="G66"/>
@@ -3105,16 +3105,16 @@
         <v>48</v>
       </c>
       <c r="B67" s="24" t="s">
+        <v>155</v>
+      </c>
+      <c r="C67" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="D67" s="25" t="s">
         <v>156</v>
       </c>
-      <c r="C67" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="D67" s="25" t="s">
+      <c r="E67" s="25" t="s">
         <v>157</v>
-      </c>
-      <c r="E67" s="25" t="s">
-        <v>158</v>
       </c>
       <c r="F67" s="29"/>
       <c r="G67"/>
@@ -3126,7 +3126,7 @@
         <v>49</v>
       </c>
       <c r="B68" s="24" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C68" s="25" t="s">
         <v>33</v>
@@ -3135,7 +3135,7 @@
         <v>139</v>
       </c>
       <c r="E68" s="25" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F68" s="29"/>
       <c r="G68"/>
@@ -3147,7 +3147,7 @@
         <v>50</v>
       </c>
       <c r="B69" s="32" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C69" s="33" t="s">
         <v>33</v>
@@ -3156,7 +3156,7 @@
         <v>101</v>
       </c>
       <c r="E69" s="33" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F69" s="34"/>
       <c r="G69"/>
@@ -3168,16 +3168,16 @@
         <v>51</v>
       </c>
       <c r="B70" s="32" t="s">
+        <v>145</v>
+      </c>
+      <c r="C70" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="D70" s="33" t="s">
         <v>146</v>
       </c>
-      <c r="C70" s="33" t="s">
-        <v>33</v>
-      </c>
-      <c r="D70" s="33" t="s">
-        <v>147</v>
-      </c>
       <c r="E70" s="33" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F70" s="34"/>
       <c r="G70"/>
@@ -3189,16 +3189,16 @@
         <v>52</v>
       </c>
       <c r="B71" s="24" t="s">
+        <v>160</v>
+      </c>
+      <c r="C71" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="D71" s="25" t="s">
         <v>161</v>
       </c>
-      <c r="C71" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="D71" s="25" t="s">
+      <c r="E71" s="25" t="s">
         <v>162</v>
-      </c>
-      <c r="E71" s="25" t="s">
-        <v>163</v>
       </c>
       <c r="F71" s="29"/>
       <c r="G71"/>
@@ -3210,16 +3210,16 @@
         <v>53</v>
       </c>
       <c r="B72" s="24" t="s">
+        <v>163</v>
+      </c>
+      <c r="C72" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="D72" s="25" t="s">
         <v>164</v>
       </c>
-      <c r="C72" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="D72" s="25" t="s">
+      <c r="E72" s="25" t="s">
         <v>165</v>
-      </c>
-      <c r="E72" s="25" t="s">
-        <v>166</v>
       </c>
       <c r="F72" s="29"/>
       <c r="G72"/>
@@ -3231,16 +3231,16 @@
         <v>54</v>
       </c>
       <c r="B73" s="24" t="s">
+        <v>166</v>
+      </c>
+      <c r="C73" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="D73" s="25" t="s">
         <v>167</v>
       </c>
-      <c r="C73" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="D73" s="25" t="s">
+      <c r="E73" s="25" t="s">
         <v>168</v>
-      </c>
-      <c r="E73" s="25" t="s">
-        <v>169</v>
       </c>
       <c r="F73" s="29"/>
       <c r="G73"/>
@@ -3252,16 +3252,16 @@
         <v>55</v>
       </c>
       <c r="B74" s="24" t="s">
+        <v>169</v>
+      </c>
+      <c r="C74" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="D74" s="25" t="s">
         <v>170</v>
       </c>
-      <c r="C74" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="D74" s="25" t="s">
+      <c r="E74" s="25" t="s">
         <v>171</v>
-      </c>
-      <c r="E74" s="25" t="s">
-        <v>172</v>
       </c>
       <c r="F74" s="29"/>
       <c r="G74"/>
@@ -3273,16 +3273,16 @@
         <v>56</v>
       </c>
       <c r="B75" s="24" t="s">
+        <v>172</v>
+      </c>
+      <c r="C75" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="D75" s="25" t="s">
         <v>173</v>
       </c>
-      <c r="C75" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="D75" s="25" t="s">
+      <c r="E75" s="25" t="s">
         <v>174</v>
-      </c>
-      <c r="E75" s="25" t="s">
-        <v>175</v>
       </c>
       <c r="F75" s="29"/>
       <c r="G75"/>
@@ -3294,16 +3294,16 @@
         <v>57</v>
       </c>
       <c r="B76" s="24" t="s">
+        <v>175</v>
+      </c>
+      <c r="C76" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="D76" s="25" t="s">
         <v>176</v>
       </c>
-      <c r="C76" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="D76" s="25" t="s">
-        <v>177</v>
-      </c>
       <c r="E76" s="25" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F76" s="29"/>
       <c r="G76"/>
@@ -3315,16 +3315,16 @@
         <v>58</v>
       </c>
       <c r="B77" s="24" t="s">
+        <v>177</v>
+      </c>
+      <c r="C77" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="D77" s="25" t="s">
         <v>178</v>
       </c>
-      <c r="C77" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="D77" s="25" t="s">
+      <c r="E77" s="25" t="s">
         <v>179</v>
-      </c>
-      <c r="E77" s="25" t="s">
-        <v>180</v>
       </c>
       <c r="F77" s="29"/>
       <c r="G77"/>
@@ -3336,16 +3336,16 @@
         <v>59</v>
       </c>
       <c r="B78" s="24" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C78" s="25" t="s">
         <v>33</v>
       </c>
       <c r="D78" s="25" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E78" s="25" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F78" s="29"/>
       <c r="G78"/>
@@ -3357,16 +3357,16 @@
         <v>60</v>
       </c>
       <c r="B79" s="24" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C79" s="25" t="s">
         <v>33</v>
       </c>
       <c r="D79" s="25" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E79" s="25" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F79" s="29"/>
       <c r="G79"/>
@@ -3378,16 +3378,16 @@
         <v>61</v>
       </c>
       <c r="B80" s="24" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C80" s="25" t="s">
         <v>33</v>
       </c>
       <c r="D80" s="25" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E80" s="25" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F80" s="29"/>
       <c r="G80"/>

</xml_diff>

<commit_message>
3.1.13 add packageTs column to telegramProcess and telegram common.
</commit_message>
<xml_diff>
--- a/meta/program/BlancoRestGeneratorTsConstants.xlsx
+++ b/meta/program/BlancoRestGeneratorTsConstants.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoRestGeneratorTs/meta/program/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63798135-8699-B54A-BB08-F2C103D3529A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9256440F-CDB3-C740-B24D-0B4305610C2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28780" yWindow="2280" windowWidth="21620" windowHeight="17540" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1049,7 +1049,7 @@
     <phoneticPr fontId="4"/>
   </si>
   <si>
-    <t>"3.1.12"</t>
+    <t>"3.1.13"</t>
     <phoneticPr fontId="4"/>
   </si>
 </sst>
@@ -1932,7 +1932,7 @@
   <dimension ref="A1:H81"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>

</xml_diff>